<commit_message>
Update Excel via browser
</commit_message>
<xml_diff>
--- a/app/data.xlsx
+++ b/app/data.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -446,9 +446,20 @@
         <v>2025-10-01T18:23:36.320Z</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>Hello</v>
+      </c>
+      <c r="B5" t="str">
+        <v>World</v>
+      </c>
+      <c r="C5" t="str">
+        <v>2025-10-01T18:27:38.913Z</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C4"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C5"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update Excel via form submission
</commit_message>
<xml_diff>
--- a/app/data.xlsx
+++ b/app/data.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -479,9 +479,23 @@
         <v>2025-10-01T18:34:25.432Z</v>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>Nara</v>
+      </c>
+      <c r="B8" t="str">
+        <v>nareay@cat.com</v>
+      </c>
+      <c r="C8" t="str">
+        <v>Employee</v>
+      </c>
+      <c r="D8" t="str">
+        <v>2025-10-01T18:37:43.378Z</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C7"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:D8"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>